<commit_message>
put all the lines inside a function for main.py to refer
</commit_message>
<xml_diff>
--- a/stock_portfolio.xlsx
+++ b/stock_portfolio.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10803"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d23262ba32bc6e2/script/python/stock_data/stock_monitor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_F25DC773A252ABDACC104825D99D687A5ADE58E4" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{40F1039C-B08D-4A84-A602-FAB37120B90D}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="11_F25DC773A252ABDACC104825D99D687A5ADE58E4" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BB41F4B9-1374-E94B-86EF-7AA1A9ECFF26}"/>
   <bookViews>
-    <workbookView xWindow="6810" yWindow="3345" windowWidth="14520" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10350" yWindow="900" windowWidth="15285" windowHeight="13725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="7">
   <si>
     <t>stock_code</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -48,14 +50,6 @@
     <t>date_in</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
-  <si>
-    <t>2/3/2020</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>29/7/2020</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
@@ -65,13 +59,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -97,11 +91,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -379,21 +374,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5078125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.98828125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5390625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,7 +402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>857</v>
       </c>
@@ -417,22 +412,50 @@
       <c r="C2">
         <v>3.14</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
+      <c r="D2" s="1">
+        <v>43892</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1912</v>
+        <v>1918</v>
       </c>
       <c r="B3">
-        <v>15000</v>
+        <v>6000</v>
       </c>
       <c r="C3">
-        <v>0.27300000000000002</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
+        <v>32.65</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>175</v>
+      </c>
+      <c r="B4">
+        <v>11000</v>
+      </c>
+      <c r="C4">
+        <v>16.18</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44082</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3883</v>
+      </c>
+      <c r="B5">
+        <v>11000</v>
+      </c>
+      <c r="C5">
+        <v>8.52</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44082</v>
       </c>
     </row>
   </sheetData>

</xml_diff>